<commit_message>
Test006 executado e Test007 preparado
</commit_message>
<xml_diff>
--- a/Python_ObstacleDetection_Model/Test0005_CrossVal_F1_Loss/Results/009_Test0005_Selected_Models_Median_Metrics/analise_modelos_selecionados.xlsx
+++ b/Python_ObstacleDetection_Model/Test0005_CrossVal_F1_Loss/Results/009_Test0005_Selected_Models_Median_Metrics/analise_modelos_selecionados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\2024_Phd_ObstacleDetectionModel\Python_ObstacleDetection_Model\Test0005_CrossVal_F1_Loss\Results\009_Test0005_Selected_Models_Median_Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053207A5-0954-4B3D-958E-C4C26A6E433E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E096D-DFB7-4690-B60E-624202152108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96B95987-A003-4425-8BAE-B4391850FCBD}"/>
   </bookViews>
@@ -262,7 +262,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{72EEBB63-909A-4835-B0D8-6495080705A7}" name="comparativo_medianas_accuracy_weighted__3" displayName="comparativo_medianas_accuracy_weighted__3" ref="A1:I14" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I14" xr:uid="{72EEBB63-909A-4835-B0D8-6495080705A7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
-    <sortCondition ref="C1:C14"/>
+    <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F9E4BE60-50C7-417B-948B-0CCA54F8872C}" uniqueName="1" name="Algoritmo" queryTableFieldId="1" dataDxfId="6"/>
@@ -599,7 +599,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,225 +647,219 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="5">
-        <v>124.55</v>
-      </c>
-      <c r="C2" s="2">
-        <v>112.65</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>120.95</v>
+      </c>
+      <c r="C2" s="3">
+        <v>118.25</v>
       </c>
       <c r="D2" s="1">
+        <v>0.94559585492227982</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.94145239464231878</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.96428571428571441</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.92777777777777781</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.9418611793611793</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.94552319309600874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.95077720207253891</v>
       </c>
-      <c r="E2" s="1">
-        <v>0.94812303037855716</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.95555006790961838</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.94444444444444442</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.94612470301162266</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.9493257820927723</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2">
-        <v>120.95</v>
-      </c>
-      <c r="C3" s="3">
-        <v>118.25</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.94559585492227982</v>
-      </c>
       <c r="E3" s="1">
-        <v>0.94145239464231878</v>
+        <v>0.94242202904564454</v>
       </c>
       <c r="F3" s="1">
-        <v>0.96428571428571441</v>
+        <v>0.96033591731266155</v>
       </c>
       <c r="G3" s="1">
         <v>0.92777777777777781</v>
       </c>
       <c r="H3" s="1">
-        <v>0.9418611793611793</v>
+        <v>0.94616718027734981</v>
       </c>
       <c r="I3" s="1">
-        <v>0.94552319309600874</v>
+        <v>0.94932578209277241</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>143.80000000000001</v>
-      </c>
-      <c r="C4" s="4">
-        <v>126.2</v>
+        <v>145.6</v>
+      </c>
+      <c r="C4">
+        <v>154.65</v>
       </c>
       <c r="D4" s="1">
-        <v>0.95336787564766845</v>
+        <v>0.94818652849740936</v>
       </c>
       <c r="E4" s="1">
-        <v>0.94933890081131977</v>
+        <v>0.94296571131510398</v>
       </c>
       <c r="F4" s="1">
-        <v>0.95427227593415198</v>
+        <v>0.95604395604395598</v>
       </c>
       <c r="G4" s="1">
-        <v>0.94444444444444442</v>
+        <v>0.9336996336996336</v>
       </c>
       <c r="H4" s="1">
-        <v>0.95027017126110436</v>
+        <v>0.94378688886784701</v>
       </c>
       <c r="I4" s="1">
-        <v>0.95315846029723805</v>
+        <v>0.94701036003149075</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>138.6</v>
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4">
+        <v>138.15</v>
       </c>
       <c r="D5" s="1">
-        <v>0.94805159758203805</v>
+        <v>0.94818652849740936</v>
       </c>
       <c r="E5" s="1">
-        <v>0.94453901457081102</v>
+        <v>0.94446640606489085</v>
       </c>
       <c r="F5" s="1">
-        <v>0.94093567251461985</v>
+        <v>0.9651162790697676</v>
       </c>
       <c r="G5" s="1">
-        <v>0.94505494505494503</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="H5" s="1">
-        <v>0.94404851212803209</v>
+        <v>0.94318181818181801</v>
       </c>
       <c r="I5" s="1">
-        <v>0.94715039862098693</v>
+        <v>0.94654800431499464</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>150.65</v>
       </c>
       <c r="C6">
-        <v>141.85</v>
+        <v>148.55000000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>0.94559585492227982</v>
+        <v>0.94818652849740936</v>
       </c>
       <c r="E6" s="1">
-        <v>0.94507609783836688</v>
+        <v>0.94452426637811238</v>
       </c>
       <c r="F6" s="1">
-        <v>0.95009881422924902</v>
+        <v>0.96491108071135434</v>
       </c>
       <c r="G6" s="1">
-        <v>0.94444444444444442</v>
+        <v>0.93333333333333324</v>
       </c>
       <c r="H6" s="1">
-        <v>0.94118385537631033</v>
+        <v>0.94350102145045955</v>
       </c>
       <c r="I6" s="1">
-        <v>0.94482200647249182</v>
+        <v>0.94689859762675299</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>159.80000000000001</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>142.35</v>
+        <v>138.6</v>
       </c>
       <c r="D7" s="1">
-        <v>0.95077720207253891</v>
+        <v>0.94805159758203805</v>
       </c>
       <c r="E7" s="1">
-        <v>0.94600129810051081</v>
+        <v>0.94453901457081102</v>
       </c>
       <c r="F7" s="1">
-        <v>0.95505617977528079</v>
+        <v>0.94093567251461985</v>
       </c>
       <c r="G7" s="1">
-        <v>0.93888888888888888</v>
+        <v>0.94505494505494503</v>
       </c>
       <c r="H7" s="1">
-        <v>0.94677044755508122</v>
+        <v>0.94404851212803209</v>
       </c>
       <c r="I7" s="1">
-        <v>0.950026968716289</v>
+        <v>0.94715039862098693</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>147.65</v>
+        <v>141.85</v>
       </c>
       <c r="D8" s="1">
-        <v>0.94818652849740936</v>
+        <v>0.94559585492227982</v>
       </c>
       <c r="E8" s="1">
-        <v>0.94578877834076014</v>
+        <v>0.94507609783836688</v>
       </c>
       <c r="F8" s="1">
-        <v>0.94680851063829796</v>
+        <v>0.95009881422924902</v>
       </c>
       <c r="G8" s="1">
-        <v>0.94505494505494503</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="H8" s="1">
-        <v>0.94413233458177281</v>
+        <v>0.94118385537631033</v>
       </c>
       <c r="I8" s="1">
-        <v>0.94759978425026969</v>
+        <v>0.94482200647249182</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>150.65</v>
-      </c>
-      <c r="C9">
-        <v>148.55000000000001</v>
+        <v>162.9</v>
       </c>
       <c r="D9" s="1">
-        <v>0.94818652849740936</v>
+        <v>0.94559585492227982</v>
       </c>
       <c r="E9" s="1">
-        <v>0.94452426637811238</v>
+        <v>0.94548067407601977</v>
       </c>
       <c r="F9" s="1">
-        <v>0.96491108071135434</v>
+        <v>0.96428571428571441</v>
       </c>
       <c r="G9" s="1">
-        <v>0.93333333333333324</v>
+        <v>0.93888888888888888</v>
       </c>
       <c r="H9" s="1">
-        <v>0.94350102145045955</v>
+        <v>0.94048154093097924</v>
       </c>
       <c r="I9" s="1">
-        <v>0.94689859762675299</v>
+        <v>0.94412081984897511</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -899,109 +893,115 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>145.6</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>154.65</v>
+        <v>147.65</v>
       </c>
       <c r="D11" s="1">
         <v>0.94818652849740936</v>
       </c>
       <c r="E11" s="1">
-        <v>0.94296571131510398</v>
+        <v>0.94578877834076014</v>
       </c>
       <c r="F11" s="1">
-        <v>0.95604395604395598</v>
+        <v>0.94680851063829796</v>
       </c>
       <c r="G11" s="1">
-        <v>0.9336996336996336</v>
+        <v>0.94505494505494503</v>
       </c>
       <c r="H11" s="1">
-        <v>0.94378688886784701</v>
+        <v>0.94413233458177281</v>
       </c>
       <c r="I11" s="1">
-        <v>0.94701036003149075</v>
+        <v>0.94759978425026969</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4">
-        <v>138.15</v>
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="C12">
+        <v>142.35</v>
       </c>
       <c r="D12" s="1">
-        <v>0.94818652849740936</v>
+        <v>0.95077720207253891</v>
       </c>
       <c r="E12" s="1">
-        <v>0.94446640606489085</v>
+        <v>0.94600129810051081</v>
       </c>
       <c r="F12" s="1">
-        <v>0.9651162790697676</v>
+        <v>0.95505617977528079</v>
       </c>
       <c r="G12" s="1">
-        <v>0.93333333333333335</v>
+        <v>0.93888888888888888</v>
       </c>
       <c r="H12" s="1">
-        <v>0.94318181818181801</v>
+        <v>0.94677044755508122</v>
       </c>
       <c r="I12" s="1">
-        <v>0.94654800431499464</v>
+        <v>0.950026968716289</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>155.30000000000001</v>
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>124.55</v>
+      </c>
+      <c r="C13" s="2">
+        <v>112.65</v>
       </c>
       <c r="D13" s="1">
         <v>0.95077720207253891</v>
       </c>
       <c r="E13" s="1">
-        <v>0.94242202904564454</v>
+        <v>0.94812303037855716</v>
       </c>
       <c r="F13" s="1">
-        <v>0.96033591731266155</v>
+        <v>0.95555006790961838</v>
       </c>
       <c r="G13" s="1">
-        <v>0.92777777777777781</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="H13" s="1">
-        <v>0.94616718027734981</v>
+        <v>0.94612470301162266</v>
       </c>
       <c r="I13" s="1">
-        <v>0.94932578209277241</v>
+        <v>0.9493257820927723</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
+      <c r="A14" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>162.9</v>
+        <v>143.80000000000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>126.2</v>
       </c>
       <c r="D14" s="1">
-        <v>0.94559585492227982</v>
+        <v>0.95336787564766845</v>
       </c>
       <c r="E14" s="1">
-        <v>0.94548067407601977</v>
+        <v>0.94933890081131977</v>
       </c>
       <c r="F14" s="1">
-        <v>0.96428571428571441</v>
+        <v>0.95427227593415198</v>
       </c>
       <c r="G14" s="1">
-        <v>0.93888888888888888</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="H14" s="1">
-        <v>0.94048154093097924</v>
+        <v>0.95027017126110436</v>
       </c>
       <c r="I14" s="1">
-        <v>0.94412081984897511</v>
+        <v>0.95315846029723805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>